<commit_message>
Assertion is added for testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Test Data.xlsx
+++ b/src/test/resources/testdata/Test Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2544F236-E09F-4A6C-BF65-B1793ED9B12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{26DA4CE7-A7E2-493C-9D0F-D3479E3932D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Opportunity Name</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>AutoOpp001</t>
+    <t>AutoOpp</t>
   </si>
   <si>
     <t>New Business</t>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>New opportunity from campaign</t>
-  </si>
-  <si>
-    <t>AutoOpp002</t>
   </si>
   <si>
     <t>Existing</t>
@@ -480,7 +477,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,31 +552,31 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>12000</v>
       </c>
       <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="2">
         <v>45879</v>
       </c>
       <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
       </c>
       <c r="H3" s="4">
         <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>